<commit_message>
changing local gskjp results to decimal numbers
</commit_message>
<xml_diff>
--- a/Projects/GSKAU_SAND/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU_SAND/Data/gsk_set_up.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Functional KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,8 +14,8 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$4</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -62,6 +62,9 @@
     <t xml:space="preserve">Include SubCategory</t>
   </si>
   <si>
+    <t xml:space="preserve">Include POSM</t>
+  </si>
+  <si>
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
@@ -71,22 +74,19 @@
     <t xml:space="preserve">Exclude</t>
   </si>
   <si>
-    <t xml:space="preserve">Oral ,Pain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adult,Child,Denture,NRT,Toothpaste,Topical,Osteo,</t>
+    <t xml:space="preserve">Adult,Child,Denture,NRT,Toothpaste,Topical,Osteo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include </t>
   </si>
   <si>
     <t xml:space="preserve">Linear SOS</t>
   </si>
   <si>
     <t xml:space="preserve">Include</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include </t>
   </si>
 </sst>
 </file>
@@ -203,7 +203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -232,28 +232,24 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -328,7 +324,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -339,33 +335,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K12" activeCellId="0" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="E20" activeCellId="0" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="56.8785425101215"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="27.2064777327935"/>
-    <col collapsed="false" hidden="false" max="1013" min="12" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1014" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -399,108 +395,92 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="ALZ1" s="0"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="26.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>12</v>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="ALZ2" s="0"/>
-      <c r="AMA2" s="0"/>
-      <c r="AMB2" s="0"/>
-      <c r="AMC2" s="0"/>
-      <c r="AMD2" s="0"/>
-      <c r="AME2" s="0"/>
-      <c r="AMF2" s="0"/>
-      <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
+      <c r="D3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>13</v>
-      </c>
+      <c r="E4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
PROS-12595-GSKAU SAND PROD Sync
</commit_message>
<xml_diff>
--- a/Projects/GSKAU_SAND/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU_SAND/Data/gsk_set_up.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Functional KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -68,7 +68,15 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf</t>
+    <t xml:space="preserve">Pain Main Shelf - Grcy
+Oral Main Shelf - Grcy
+NRT Main Shelf - Grcy
+Counter Unit - Grcy
+Floor Bin - Grcy
+Gondola End - Grcy
+Hangsell - Grcy
+Clipstrip - Grcy
+Hotspot Tray – Grcy</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -96,7 +104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,12 +141,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -203,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,15 +246,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -342,24 +340,24 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L4" activeCellId="0" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.1740890688259"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
@@ -403,7 +401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -429,11 +427,11 @@
       <c r="K2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -456,8 +454,8 @@
       <c r="H3" s="0"/>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="12" t="s">
+      <c r="K3" s="10"/>
+      <c r="L3" s="11" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PROS-12595 GSKAU-SAND template update
</commit_message>
<xml_diff>
--- a/Projects/GSKAU_SAND/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU_SAND/Data/gsk_set_up.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -68,14 +68,14 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain Main Shelf - Grcy
-Oral Main Shelf - Grcy
-NRT Main Shelf - Grcy
-Counter Unit - Grcy
-Floor Bin - Grcy
-Gondola End - Grcy
-Hangsell - Grcy
-Clipstrip - Grcy
+    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf - Grcy,
+Oral Main Shelf - Grcy,
+NRT Main Shelf - Grcy,
+Counter Unit - Grcy,
+Floor Bin - Grcy,
+Gondola End - Grcy,
+Hangsell - Grcy,
+Clipstrip - Grcy,
 Hotspot Tray – Grcy</t>
   </si>
   <si>
@@ -326,7 +326,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -344,20 +344,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
@@ -401,7 +401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="326.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -431,7 +431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="164.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
GSKAU Sand Env setup file update
</commit_message>
<xml_diff>
--- a/Projects/GSKAU_SAND/Data/gsk_set_up.xlsx
+++ b/Projects/GSKAU_SAND/Data/gsk_set_up.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -68,15 +68,9 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf - Grcy,
-Oral Main Shelf - Grcy,
-NRT Main Shelf - Grcy,
-Counter Unit - Grcy,
-Floor Bin - Grcy,
-Gondola End - Grcy,
-Hangsell - Grcy,
-Clipstrip - Grcy,
-Hotspot Tray – Grcy</t>
+    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf,Pain Main Shelf – Grcy,
+Oral Main Shelf – Grcy,
+NRT Main Shelf – Grcy</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -326,7 +320,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -344,26 +338,28 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1014" min="13" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="51.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -401,7 +397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="5" customFormat="true" ht="326.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="74.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -431,7 +427,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="164.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>17</v>
       </c>
@@ -459,7 +455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>